<commit_message>
Created Summary for Peak,Non-Peak
</commit_message>
<xml_diff>
--- a/Data/Intersection Data/Corrales - JR Borja/TVC Summary.xlsx
+++ b/Data/Intersection Data/Corrales - JR Borja/TVC Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Gthub Repo\Genetic_Fuzzy_Algo\Data\Intersection Data\Corrales - JR Borja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\IOT CODING SHIT\XUTrafficSignalOptimization2122\Data\Intersection Data\Corrales - JR Borja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7B6D7E-62A6-4233-B4B6-84BB73859DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FB1AA5-1799-40EC-981A-B1E09A23C0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A139AC8C-9445-4167-B3D6-D99F9ED15635}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="862" activeTab="10" xr2:uid="{A139AC8C-9445-4167-B3D6-D99F9ED15635}"/>
   </bookViews>
   <sheets>
     <sheet name="North_West" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,11 @@
     <sheet name="West_East" sheetId="8" r:id="rId6"/>
     <sheet name="East_North" sheetId="3" r:id="rId7"/>
     <sheet name="East_West" sheetId="4" r:id="rId8"/>
+    <sheet name="Per Hour Total" sheetId="9" r:id="rId9"/>
+    <sheet name="Peak Hour Summary" sheetId="11" r:id="rId10"/>
+    <sheet name="Non-Peak Hour Summary" sheetId="12" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,8 +33,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="54">
   <si>
     <t>Time</t>
   </si>
@@ -121,12 +127,93 @@
   <si>
     <t>others</t>
   </si>
+  <si>
+    <t>North_South</t>
+  </si>
+  <si>
+    <t>North_West</t>
+  </si>
+  <si>
+    <t>South_East</t>
+  </si>
+  <si>
+    <t>South_North</t>
+  </si>
+  <si>
+    <t>West_South</t>
+  </si>
+  <si>
+    <t>West_East</t>
+  </si>
+  <si>
+    <t>East_North</t>
+  </si>
+  <si>
+    <t>East_West</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Largest</t>
+  </si>
+  <si>
+    <t>Smallest</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Non-Peak</t>
+  </si>
+  <si>
+    <t>Peak</t>
+  </si>
+  <si>
+    <t>AM Peak Hour</t>
+  </si>
+  <si>
+    <t>8:00-9:00am</t>
+  </si>
+  <si>
+    <t>PM Peak Hour</t>
+  </si>
+  <si>
+    <t>3:00-4:00pm</t>
+  </si>
+  <si>
+    <t>AM Non-Peak Hour</t>
+  </si>
+  <si>
+    <t>5:00-6:00am</t>
+  </si>
+  <si>
+    <t>PM Non-Peak Hour</t>
+  </si>
+  <si>
+    <t>PCU Factors:</t>
+  </si>
+  <si>
+    <t>PCEF:</t>
+  </si>
+  <si>
+    <t>In PCEF:</t>
+  </si>
+  <si>
+    <t>7:00-8:00pm</t>
+  </si>
+  <si>
+    <t>In PCEF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,8 +251,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +278,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -245,11 +357,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -304,6 +455,69 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D1911B-6375-4D3D-A628-E8315C57D9D4}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1190,12 +1404,3368 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B49315D-0F6D-4940-95A4-B7397DCC8B16}">
+  <dimension ref="A1:X27"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:X12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="10" width="14.33203125" customWidth="1"/>
+    <col min="23" max="23" width="16.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="38"/>
+    </row>
+    <row r="3" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="22">
+        <v>116</v>
+      </c>
+      <c r="C3" s="22">
+        <v>167</v>
+      </c>
+      <c r="D3" s="22">
+        <v>17</v>
+      </c>
+      <c r="E3" s="22">
+        <v>254</v>
+      </c>
+      <c r="F3" s="22">
+        <v>2</v>
+      </c>
+      <c r="G3" s="22">
+        <v>75</v>
+      </c>
+      <c r="H3" s="22">
+        <v>26</v>
+      </c>
+      <c r="I3" s="22">
+        <v>85</v>
+      </c>
+      <c r="J3" s="29">
+        <f>SUM(B3:I3)</f>
+        <v>742</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="22">
+        <f>B3*$X3</f>
+        <v>116</v>
+      </c>
+      <c r="N3" s="22">
+        <f t="shared" ref="N3:T3" si="0">C3*$X3</f>
+        <v>167</v>
+      </c>
+      <c r="O3" s="22">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P3" s="22">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="Q3" s="22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R3" s="22">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="S3" s="22">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="T3" s="22">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="U3" s="29">
+        <f>SUM(M3:T3)</f>
+        <v>742</v>
+      </c>
+      <c r="V3" s="38"/>
+      <c r="W3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="X3" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="22">
+        <v>143</v>
+      </c>
+      <c r="C4" s="22">
+        <v>70</v>
+      </c>
+      <c r="D4" s="22">
+        <v>10</v>
+      </c>
+      <c r="E4" s="22">
+        <v>162</v>
+      </c>
+      <c r="F4" s="22">
+        <v>6</v>
+      </c>
+      <c r="G4" s="22">
+        <v>136</v>
+      </c>
+      <c r="H4" s="22">
+        <v>19</v>
+      </c>
+      <c r="I4" s="22">
+        <v>90</v>
+      </c>
+      <c r="J4" s="29">
+        <f t="shared" ref="J4:J12" si="1">SUM(B4:I4)</f>
+        <v>636</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="22">
+        <f t="shared" ref="M4:M12" si="2">B4*$X4</f>
+        <v>71.5</v>
+      </c>
+      <c r="N4" s="22">
+        <f t="shared" ref="N4:N12" si="3">C4*$X4</f>
+        <v>35</v>
+      </c>
+      <c r="O4" s="22">
+        <f t="shared" ref="O4:O12" si="4">D4*$X4</f>
+        <v>5</v>
+      </c>
+      <c r="P4" s="22">
+        <f t="shared" ref="P4:P12" si="5">E4*$X4</f>
+        <v>81</v>
+      </c>
+      <c r="Q4" s="22">
+        <f t="shared" ref="Q4:Q12" si="6">F4*$X4</f>
+        <v>3</v>
+      </c>
+      <c r="R4" s="22">
+        <f t="shared" ref="R4:R12" si="7">G4*$X4</f>
+        <v>68</v>
+      </c>
+      <c r="S4" s="22">
+        <f t="shared" ref="S4:S12" si="8">H4*$X4</f>
+        <v>9.5</v>
+      </c>
+      <c r="T4" s="22">
+        <f t="shared" ref="T4:T12" si="9">I4*$X4</f>
+        <v>45</v>
+      </c>
+      <c r="U4" s="29">
+        <f t="shared" ref="U4:U12" si="10">SUM(M4:T4)</f>
+        <v>318</v>
+      </c>
+      <c r="V4" s="38"/>
+      <c r="W4" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="22">
+        <v>27</v>
+      </c>
+      <c r="C5" s="22">
+        <v>62</v>
+      </c>
+      <c r="D5" s="22">
+        <v>2</v>
+      </c>
+      <c r="E5" s="22">
+        <v>79</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22">
+        <v>14</v>
+      </c>
+      <c r="H5" s="22">
+        <v>10</v>
+      </c>
+      <c r="I5" s="22">
+        <v>26</v>
+      </c>
+      <c r="J5" s="29">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="22">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N5" s="22">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="O5" s="22">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="P5" s="22">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="Q5" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="22">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="S5" s="22">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="T5" s="22">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="U5" s="29">
+        <f t="shared" si="10"/>
+        <v>220</v>
+      </c>
+      <c r="V5" s="38"/>
+      <c r="W5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="X5" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30">
+        <v>1</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q6" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="29">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="V6" s="38"/>
+      <c r="W6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="X6" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="22">
+        <v>6</v>
+      </c>
+      <c r="C7" s="22">
+        <v>5</v>
+      </c>
+      <c r="D7" s="22">
+        <v>1</v>
+      </c>
+      <c r="E7" s="22">
+        <v>10</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22">
+        <v>2</v>
+      </c>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22">
+        <v>11</v>
+      </c>
+      <c r="J7" s="29">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="22">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N7" s="22">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="O7" s="22">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="P7" s="22">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="Q7" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="22">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="S7" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="22">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="U7" s="29">
+        <f t="shared" si="10"/>
+        <v>70</v>
+      </c>
+      <c r="V7" s="38"/>
+      <c r="W7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="X7" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="29">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="38"/>
+      <c r="W8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="X8" s="39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="22">
+        <v>9</v>
+      </c>
+      <c r="C9" s="22">
+        <v>4</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="29">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="22">
+        <f t="shared" si="2"/>
+        <v>22.5</v>
+      </c>
+      <c r="N9" s="22">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="O9" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="29">
+        <f t="shared" si="10"/>
+        <v>32.5</v>
+      </c>
+      <c r="V9" s="38"/>
+      <c r="W9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="X9" s="39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30">
+        <v>41</v>
+      </c>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30">
+        <v>173</v>
+      </c>
+      <c r="J10" s="29">
+        <f t="shared" si="1"/>
+        <v>214</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="22">
+        <f t="shared" si="5"/>
+        <v>61.5</v>
+      </c>
+      <c r="Q10" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S10" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T10" s="22">
+        <f t="shared" si="9"/>
+        <v>259.5</v>
+      </c>
+      <c r="U10" s="29">
+        <f t="shared" si="10"/>
+        <v>321</v>
+      </c>
+      <c r="V10" s="38"/>
+      <c r="W10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="X10" s="39">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="22">
+        <v>236</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22">
+        <v>11</v>
+      </c>
+      <c r="E11" s="22">
+        <v>183</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22">
+        <v>137</v>
+      </c>
+      <c r="H11" s="22">
+        <v>31</v>
+      </c>
+      <c r="I11" s="22">
+        <v>257</v>
+      </c>
+      <c r="J11" s="29">
+        <f t="shared" si="1"/>
+        <v>855</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="22">
+        <f t="shared" si="2"/>
+        <v>590</v>
+      </c>
+      <c r="N11" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="22">
+        <f t="shared" si="4"/>
+        <v>27.5</v>
+      </c>
+      <c r="P11" s="22">
+        <f t="shared" si="5"/>
+        <v>457.5</v>
+      </c>
+      <c r="Q11" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="22">
+        <f t="shared" si="7"/>
+        <v>342.5</v>
+      </c>
+      <c r="S11" s="22">
+        <f t="shared" si="8"/>
+        <v>77.5</v>
+      </c>
+      <c r="T11" s="22">
+        <f t="shared" si="9"/>
+        <v>642.5</v>
+      </c>
+      <c r="U11" s="29">
+        <f t="shared" si="10"/>
+        <v>2137.5</v>
+      </c>
+      <c r="V11" s="38"/>
+      <c r="W11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="X11" s="39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="22">
+        <v>7</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22">
+        <v>3</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22">
+        <v>14</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22">
+        <v>12</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="22">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N12" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="22">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="Q12" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="22">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="S12" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T12" s="22">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="U12" s="29">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+      <c r="V12" s="38"/>
+      <c r="W12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="X12" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19">
+        <f>SUM(B3:B12)</f>
+        <v>544</v>
+      </c>
+      <c r="C13" s="19">
+        <f t="shared" ref="C13:J13" si="11">SUM(C3:C12)</f>
+        <v>308</v>
+      </c>
+      <c r="D13" s="19">
+        <f t="shared" si="11"/>
+        <v>41</v>
+      </c>
+      <c r="E13" s="19">
+        <f t="shared" si="11"/>
+        <v>733</v>
+      </c>
+      <c r="F13" s="19">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="19">
+        <f t="shared" si="11"/>
+        <v>378</v>
+      </c>
+      <c r="H13" s="19">
+        <f t="shared" si="11"/>
+        <v>86</v>
+      </c>
+      <c r="I13" s="19">
+        <f t="shared" si="11"/>
+        <v>654</v>
+      </c>
+      <c r="J13" s="19">
+        <f t="shared" si="11"/>
+        <v>2752</v>
+      </c>
+      <c r="M13" s="19">
+        <f>SUM(M3:M12)</f>
+        <v>846</v>
+      </c>
+      <c r="N13" s="19">
+        <f t="shared" ref="N13:U13" si="12">SUM(N3:N12)</f>
+        <v>284</v>
+      </c>
+      <c r="O13" s="19">
+        <f t="shared" si="12"/>
+        <v>53.5</v>
+      </c>
+      <c r="P13" s="19">
+        <f t="shared" si="12"/>
+        <v>958</v>
+      </c>
+      <c r="Q13" s="19">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="R13" s="19">
+        <f t="shared" si="12"/>
+        <v>517.5</v>
+      </c>
+      <c r="S13" s="19">
+        <f t="shared" si="12"/>
+        <v>123</v>
+      </c>
+      <c r="T13" s="19">
+        <f t="shared" si="12"/>
+        <v>1092</v>
+      </c>
+      <c r="U13" s="19">
+        <f t="shared" si="12"/>
+        <v>3879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="31"/>
+      <c r="B16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="S16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="T16" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U16" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="V16" s="38"/>
+    </row>
+    <row r="17" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="22">
+        <v>153</v>
+      </c>
+      <c r="C17" s="22">
+        <v>229</v>
+      </c>
+      <c r="D17" s="22">
+        <v>18</v>
+      </c>
+      <c r="E17" s="22">
+        <v>320</v>
+      </c>
+      <c r="F17" s="22">
+        <v>2</v>
+      </c>
+      <c r="G17" s="22">
+        <v>88</v>
+      </c>
+      <c r="H17" s="22">
+        <v>14</v>
+      </c>
+      <c r="I17" s="22">
+        <v>97</v>
+      </c>
+      <c r="J17" s="19">
+        <f>SUM(B17:I17)</f>
+        <v>921</v>
+      </c>
+      <c r="L17" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="22">
+        <f>B17*$X3</f>
+        <v>153</v>
+      </c>
+      <c r="N17" s="22">
+        <f t="shared" ref="N17:T17" si="13">C17*$X3</f>
+        <v>229</v>
+      </c>
+      <c r="O17" s="22">
+        <f t="shared" si="13"/>
+        <v>18</v>
+      </c>
+      <c r="P17" s="22">
+        <f t="shared" si="13"/>
+        <v>320</v>
+      </c>
+      <c r="Q17" s="22">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="R17" s="22">
+        <f t="shared" si="13"/>
+        <v>88</v>
+      </c>
+      <c r="S17" s="22">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="T17" s="22">
+        <f t="shared" si="13"/>
+        <v>97</v>
+      </c>
+      <c r="U17" s="29">
+        <f>SUM(M17:T17)</f>
+        <v>921</v>
+      </c>
+      <c r="V17" s="38"/>
+    </row>
+    <row r="18" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="22">
+        <v>178</v>
+      </c>
+      <c r="C18" s="22">
+        <v>117</v>
+      </c>
+      <c r="D18" s="22">
+        <v>13</v>
+      </c>
+      <c r="E18" s="22">
+        <v>138</v>
+      </c>
+      <c r="F18" s="22">
+        <v>9</v>
+      </c>
+      <c r="G18" s="22">
+        <v>110</v>
+      </c>
+      <c r="H18" s="22">
+        <v>30</v>
+      </c>
+      <c r="I18" s="22">
+        <v>101</v>
+      </c>
+      <c r="J18" s="19">
+        <f t="shared" ref="J18:J27" si="14">SUM(B18:I18)</f>
+        <v>696</v>
+      </c>
+      <c r="L18" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="22">
+        <f t="shared" ref="M18:M26" si="15">B18*$X4</f>
+        <v>89</v>
+      </c>
+      <c r="N18" s="22">
+        <f t="shared" ref="N18:N26" si="16">C18*$X4</f>
+        <v>58.5</v>
+      </c>
+      <c r="O18" s="22">
+        <f t="shared" ref="O18:O26" si="17">D18*$X4</f>
+        <v>6.5</v>
+      </c>
+      <c r="P18" s="22">
+        <f t="shared" ref="P18:P26" si="18">E18*$X4</f>
+        <v>69</v>
+      </c>
+      <c r="Q18" s="22">
+        <f t="shared" ref="Q18:Q26" si="19">F18*$X4</f>
+        <v>4.5</v>
+      </c>
+      <c r="R18" s="22">
+        <f t="shared" ref="R18:R26" si="20">G18*$X4</f>
+        <v>55</v>
+      </c>
+      <c r="S18" s="22">
+        <f t="shared" ref="S18:S26" si="21">H18*$X4</f>
+        <v>15</v>
+      </c>
+      <c r="T18" s="22">
+        <f t="shared" ref="T18:T26" si="22">I18*$X4</f>
+        <v>50.5</v>
+      </c>
+      <c r="U18" s="29">
+        <f t="shared" ref="U18:U26" si="23">SUM(M18:T18)</f>
+        <v>348</v>
+      </c>
+      <c r="V18" s="38"/>
+    </row>
+    <row r="19" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="22">
+        <v>22</v>
+      </c>
+      <c r="C19" s="22">
+        <v>59</v>
+      </c>
+      <c r="D19" s="22">
+        <v>1</v>
+      </c>
+      <c r="E19" s="22">
+        <v>115</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22">
+        <v>13</v>
+      </c>
+      <c r="H19" s="22">
+        <v>14</v>
+      </c>
+      <c r="I19" s="22">
+        <v>41</v>
+      </c>
+      <c r="J19" s="19">
+        <f t="shared" si="14"/>
+        <v>265</v>
+      </c>
+      <c r="L19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="22">
+        <f t="shared" si="15"/>
+        <v>22</v>
+      </c>
+      <c r="N19" s="22">
+        <f t="shared" si="16"/>
+        <v>59</v>
+      </c>
+      <c r="O19" s="22">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="P19" s="22">
+        <f t="shared" si="18"/>
+        <v>115</v>
+      </c>
+      <c r="Q19" s="22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="22">
+        <f t="shared" si="20"/>
+        <v>13</v>
+      </c>
+      <c r="S19" s="22">
+        <f t="shared" si="21"/>
+        <v>14</v>
+      </c>
+      <c r="T19" s="22">
+        <f t="shared" si="22"/>
+        <v>41</v>
+      </c>
+      <c r="U19" s="29">
+        <f t="shared" si="23"/>
+        <v>265</v>
+      </c>
+      <c r="V19" s="38"/>
+    </row>
+    <row r="20" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30">
+        <v>4</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="19">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="L20" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="22">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="O20" s="22">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="22">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="22">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S20" s="22">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="22">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="29">
+        <f t="shared" si="23"/>
+        <v>8</v>
+      </c>
+      <c r="V20" s="38"/>
+    </row>
+    <row r="21" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="22">
+        <v>9</v>
+      </c>
+      <c r="C21" s="22">
+        <v>10</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22">
+        <v>3</v>
+      </c>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22">
+        <v>11</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22">
+        <v>16</v>
+      </c>
+      <c r="J21" s="19">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="L21" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="22">
+        <f t="shared" si="15"/>
+        <v>18</v>
+      </c>
+      <c r="N21" s="22">
+        <f t="shared" si="16"/>
+        <v>20</v>
+      </c>
+      <c r="O21" s="22">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="22">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="Q21" s="22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="22">
+        <f t="shared" si="20"/>
+        <v>22</v>
+      </c>
+      <c r="S21" s="22">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T21" s="22">
+        <f t="shared" si="22"/>
+        <v>32</v>
+      </c>
+      <c r="U21" s="29">
+        <f t="shared" si="23"/>
+        <v>98</v>
+      </c>
+      <c r="V21" s="38"/>
+    </row>
+    <row r="22" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30">
+        <v>2</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30">
+        <v>3</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="19">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="L22" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="22">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="O22" s="22">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="22">
+        <f t="shared" si="18"/>
+        <v>7.5</v>
+      </c>
+      <c r="Q22" s="22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="22">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S22" s="22">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="22">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="29">
+        <f t="shared" si="23"/>
+        <v>12.5</v>
+      </c>
+      <c r="V22" s="38"/>
+    </row>
+    <row r="23" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="22">
+        <v>6</v>
+      </c>
+      <c r="C23" s="22">
+        <v>5</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="19">
+        <f t="shared" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="22">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="N23" s="22">
+        <f t="shared" si="16"/>
+        <v>12.5</v>
+      </c>
+      <c r="O23" s="22">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="22">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="22">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="22">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="22">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="29">
+        <f t="shared" si="23"/>
+        <v>27.5</v>
+      </c>
+      <c r="V23" s="38"/>
+    </row>
+    <row r="24" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30">
+        <v>18</v>
+      </c>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30">
+        <v>1</v>
+      </c>
+      <c r="H24" s="30">
+        <v>3</v>
+      </c>
+      <c r="I24" s="30">
+        <v>75</v>
+      </c>
+      <c r="J24" s="19">
+        <f t="shared" si="14"/>
+        <v>97</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="22">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="22">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="22">
+        <f t="shared" si="18"/>
+        <v>27</v>
+      </c>
+      <c r="Q24" s="22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="22">
+        <f t="shared" si="20"/>
+        <v>1.5</v>
+      </c>
+      <c r="S24" s="22">
+        <f t="shared" si="21"/>
+        <v>4.5</v>
+      </c>
+      <c r="T24" s="22">
+        <f t="shared" si="22"/>
+        <v>112.5</v>
+      </c>
+      <c r="U24" s="29">
+        <f t="shared" si="23"/>
+        <v>145.5</v>
+      </c>
+      <c r="V24" s="38"/>
+    </row>
+    <row r="25" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="22">
+        <v>160</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22">
+        <v>10</v>
+      </c>
+      <c r="E25" s="22">
+        <v>144</v>
+      </c>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22">
+        <v>129</v>
+      </c>
+      <c r="H25" s="22">
+        <v>60</v>
+      </c>
+      <c r="I25" s="22">
+        <v>152</v>
+      </c>
+      <c r="J25" s="19">
+        <f t="shared" si="14"/>
+        <v>655</v>
+      </c>
+      <c r="L25" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="22">
+        <f t="shared" si="15"/>
+        <v>400</v>
+      </c>
+      <c r="N25" s="22">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="22">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="P25" s="22">
+        <f t="shared" si="18"/>
+        <v>360</v>
+      </c>
+      <c r="Q25" s="22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="22">
+        <f t="shared" si="20"/>
+        <v>322.5</v>
+      </c>
+      <c r="S25" s="22">
+        <f t="shared" si="21"/>
+        <v>150</v>
+      </c>
+      <c r="T25" s="22">
+        <f t="shared" si="22"/>
+        <v>380</v>
+      </c>
+      <c r="U25" s="29">
+        <f t="shared" si="23"/>
+        <v>1637.5</v>
+      </c>
+      <c r="V25" s="38"/>
+    </row>
+    <row r="26" spans="1:22" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="22">
+        <v>1</v>
+      </c>
+      <c r="C26" s="22">
+        <v>4</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22">
+        <v>1</v>
+      </c>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22">
+        <v>3</v>
+      </c>
+      <c r="H26" s="22">
+        <v>2</v>
+      </c>
+      <c r="I26" s="22">
+        <v>4</v>
+      </c>
+      <c r="J26" s="19">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="L26" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="22">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="N26" s="22">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="O26" s="22">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="22">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="Q26" s="22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="22">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="S26" s="22">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="T26" s="22">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="U26" s="29">
+        <f t="shared" si="23"/>
+        <v>15</v>
+      </c>
+      <c r="V26" s="38"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19">
+        <f>SUM(B17:B26)</f>
+        <v>529</v>
+      </c>
+      <c r="C27" s="19">
+        <f t="shared" ref="C27:I27" si="24">SUM(C17:C26)</f>
+        <v>430</v>
+      </c>
+      <c r="D27" s="19">
+        <f t="shared" si="24"/>
+        <v>42</v>
+      </c>
+      <c r="E27" s="19">
+        <f t="shared" si="24"/>
+        <v>742</v>
+      </c>
+      <c r="F27" s="19">
+        <f t="shared" si="24"/>
+        <v>11</v>
+      </c>
+      <c r="G27" s="19">
+        <f t="shared" si="24"/>
+        <v>355</v>
+      </c>
+      <c r="H27" s="19">
+        <f t="shared" si="24"/>
+        <v>123</v>
+      </c>
+      <c r="I27" s="19">
+        <f t="shared" si="24"/>
+        <v>486</v>
+      </c>
+      <c r="J27" s="19">
+        <f t="shared" si="14"/>
+        <v>2718</v>
+      </c>
+      <c r="M27" s="19">
+        <f>SUM(M17:M26)</f>
+        <v>698</v>
+      </c>
+      <c r="N27" s="19">
+        <f t="shared" ref="N27:U27" si="25">SUM(N17:N26)</f>
+        <v>396</v>
+      </c>
+      <c r="O27" s="19">
+        <f t="shared" si="25"/>
+        <v>50.5</v>
+      </c>
+      <c r="P27" s="19">
+        <f t="shared" si="25"/>
+        <v>905.5</v>
+      </c>
+      <c r="Q27" s="19">
+        <f t="shared" si="25"/>
+        <v>6.5</v>
+      </c>
+      <c r="R27" s="19">
+        <f t="shared" si="25"/>
+        <v>505</v>
+      </c>
+      <c r="S27" s="19">
+        <f t="shared" si="25"/>
+        <v>199.5</v>
+      </c>
+      <c r="T27" s="19">
+        <f t="shared" si="25"/>
+        <v>717</v>
+      </c>
+      <c r="U27" s="19">
+        <f t="shared" si="25"/>
+        <v>3478</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB4D613-DDD2-4898-A13C-B7936D32E891}">
+  <dimension ref="A1:X27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="10" width="13.77734375" customWidth="1"/>
+    <col min="12" max="21" width="10.88671875" customWidth="1"/>
+    <col min="23" max="23" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="24">
+        <v>13</v>
+      </c>
+      <c r="C3" s="24">
+        <v>27</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24">
+        <v>35</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24">
+        <v>5</v>
+      </c>
+      <c r="H3" s="24">
+        <v>3</v>
+      </c>
+      <c r="I3" s="24">
+        <v>9</v>
+      </c>
+      <c r="J3" s="29">
+        <f>SUM(B3:I3)</f>
+        <v>92</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="24">
+        <f>B3*$X3</f>
+        <v>13</v>
+      </c>
+      <c r="N3" s="24">
+        <f t="shared" ref="N3:T3" si="0">C3*$X3</f>
+        <v>27</v>
+      </c>
+      <c r="O3" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="24">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="Q3" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="S3" s="24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="T3" s="24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="U3" s="29">
+        <f>SUM(M3:T3)</f>
+        <v>92</v>
+      </c>
+      <c r="W3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="X3" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="24">
+        <v>19</v>
+      </c>
+      <c r="C4" s="24">
+        <v>18</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24">
+        <v>60</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24">
+        <v>22</v>
+      </c>
+      <c r="H4" s="24">
+        <v>3</v>
+      </c>
+      <c r="I4" s="24">
+        <v>30</v>
+      </c>
+      <c r="J4" s="29">
+        <f t="shared" ref="J4:J12" si="1">SUM(B4:I4)</f>
+        <v>152</v>
+      </c>
+      <c r="L4" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="24">
+        <f t="shared" ref="M4:M12" si="2">B4*$X4</f>
+        <v>9.5</v>
+      </c>
+      <c r="N4" s="24">
+        <f t="shared" ref="N4:N12" si="3">C4*$X4</f>
+        <v>9</v>
+      </c>
+      <c r="O4" s="24">
+        <f t="shared" ref="O4:O12" si="4">D4*$X4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="24">
+        <f t="shared" ref="P4:P12" si="5">E4*$X4</f>
+        <v>30</v>
+      </c>
+      <c r="Q4" s="24">
+        <f t="shared" ref="Q4:Q12" si="6">F4*$X4</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="24">
+        <f t="shared" ref="R4:R12" si="7">G4*$X4</f>
+        <v>11</v>
+      </c>
+      <c r="S4" s="24">
+        <f t="shared" ref="S4:S12" si="8">H4*$X4</f>
+        <v>1.5</v>
+      </c>
+      <c r="T4" s="24">
+        <f t="shared" ref="T4:T12" si="9">I4*$X4</f>
+        <v>15</v>
+      </c>
+      <c r="U4" s="29">
+        <f t="shared" ref="U4:U13" si="10">SUM(M4:T4)</f>
+        <v>76</v>
+      </c>
+      <c r="W4" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="24">
+        <v>4</v>
+      </c>
+      <c r="C5" s="24">
+        <v>15</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24">
+        <v>35</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24">
+        <v>5</v>
+      </c>
+      <c r="H5" s="24">
+        <v>1</v>
+      </c>
+      <c r="I5" s="24">
+        <v>2</v>
+      </c>
+      <c r="J5" s="29">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="24">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N5" s="24">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="O5" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="24">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="Q5" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="24">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="S5" s="24">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T5" s="24">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="U5" s="29">
+        <f t="shared" si="10"/>
+        <v>62</v>
+      </c>
+      <c r="W5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="X5" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36">
+        <v>1</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36">
+        <v>2</v>
+      </c>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="29">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="O6" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="24">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="Q6" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="29">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="W6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="X6" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="24">
+        <v>2</v>
+      </c>
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24">
+        <v>3</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24">
+        <v>1</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="29">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="24">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N7" s="24">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="O7" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="24">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="Q7" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="24">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="S7" s="24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="29">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="W7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="X7" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36">
+        <v>1</v>
+      </c>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="24">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="Q8" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="29">
+        <f t="shared" si="10"/>
+        <v>2.5</v>
+      </c>
+      <c r="W8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="X8" s="39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="24">
+        <v>2</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="29">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="24">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N9" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="29">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="W9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="X9" s="39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36">
+        <v>16</v>
+      </c>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36">
+        <v>1</v>
+      </c>
+      <c r="H10" s="36">
+        <v>1</v>
+      </c>
+      <c r="I10" s="36">
+        <v>28</v>
+      </c>
+      <c r="J10" s="29">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="24">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="Q10" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="24">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="S10" s="24">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="T10" s="24">
+        <f t="shared" si="9"/>
+        <v>42</v>
+      </c>
+      <c r="U10" s="29">
+        <f t="shared" si="10"/>
+        <v>69</v>
+      </c>
+      <c r="W10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="X10" s="39">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="24">
+        <v>44</v>
+      </c>
+      <c r="C11" s="24">
+        <v>2</v>
+      </c>
+      <c r="D11" s="24">
+        <v>2</v>
+      </c>
+      <c r="E11" s="24">
+        <v>41</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24">
+        <v>59</v>
+      </c>
+      <c r="H11" s="24">
+        <v>7</v>
+      </c>
+      <c r="I11" s="24">
+        <v>68</v>
+      </c>
+      <c r="J11" s="29">
+        <f t="shared" si="1"/>
+        <v>223</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="24">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="N11" s="24">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="O11" s="24">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="P11" s="24">
+        <f t="shared" si="5"/>
+        <v>102.5</v>
+      </c>
+      <c r="Q11" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="24">
+        <f t="shared" si="7"/>
+        <v>147.5</v>
+      </c>
+      <c r="S11" s="24">
+        <f t="shared" si="8"/>
+        <v>17.5</v>
+      </c>
+      <c r="T11" s="24">
+        <f t="shared" si="9"/>
+        <v>170</v>
+      </c>
+      <c r="U11" s="29">
+        <f t="shared" si="10"/>
+        <v>557.5</v>
+      </c>
+      <c r="W11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="X11" s="39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="24">
+        <v>1</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24">
+        <v>8</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24">
+        <v>4</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="24">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="S12" s="24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T12" s="24">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="U12" s="29">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="W12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="X12" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19">
+        <f>SUM(B3:B12)</f>
+        <v>85</v>
+      </c>
+      <c r="C13" s="19">
+        <f t="shared" ref="C13:J13" si="11">SUM(C3:C12)</f>
+        <v>64</v>
+      </c>
+      <c r="D13" s="19">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="19">
+        <f t="shared" si="11"/>
+        <v>193</v>
+      </c>
+      <c r="F13" s="19">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="19">
+        <f t="shared" si="11"/>
+        <v>101</v>
+      </c>
+      <c r="H13" s="19">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="I13" s="19">
+        <f t="shared" si="11"/>
+        <v>141</v>
+      </c>
+      <c r="J13" s="19">
+        <f t="shared" si="11"/>
+        <v>601</v>
+      </c>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19">
+        <f>SUM(M3:M12)</f>
+        <v>146.5</v>
+      </c>
+      <c r="N13" s="19">
+        <f t="shared" ref="N13:T13" si="12">SUM(N3:N12)</f>
+        <v>60</v>
+      </c>
+      <c r="O13" s="19">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="P13" s="19">
+        <f t="shared" si="12"/>
+        <v>239</v>
+      </c>
+      <c r="Q13" s="19">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="19">
+        <f t="shared" si="12"/>
+        <v>180</v>
+      </c>
+      <c r="S13" s="19">
+        <f t="shared" si="12"/>
+        <v>24.5</v>
+      </c>
+      <c r="T13" s="19">
+        <f t="shared" si="12"/>
+        <v>242</v>
+      </c>
+      <c r="U13" s="29">
+        <f t="shared" si="10"/>
+        <v>897</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="31"/>
+      <c r="B16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="R16" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="S16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="T16" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U16" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="24">
+        <v>87</v>
+      </c>
+      <c r="C17" s="24">
+        <v>304</v>
+      </c>
+      <c r="D17" s="24">
+        <v>7</v>
+      </c>
+      <c r="E17" s="24">
+        <v>165</v>
+      </c>
+      <c r="F17" s="24">
+        <v>3</v>
+      </c>
+      <c r="G17" s="24">
+        <v>45</v>
+      </c>
+      <c r="H17" s="24">
+        <v>4</v>
+      </c>
+      <c r="I17" s="24">
+        <v>47</v>
+      </c>
+      <c r="J17" s="19">
+        <f>SUM(B17:I17)</f>
+        <v>662</v>
+      </c>
+      <c r="L17" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="24">
+        <f>B17*$X3</f>
+        <v>87</v>
+      </c>
+      <c r="N17" s="24">
+        <f t="shared" ref="N17:T26" si="13">C17*$X3</f>
+        <v>304</v>
+      </c>
+      <c r="O17" s="24">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="P17" s="24">
+        <f t="shared" si="13"/>
+        <v>165</v>
+      </c>
+      <c r="Q17" s="24">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="R17" s="24">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="S17" s="24">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="T17" s="24">
+        <f t="shared" si="13"/>
+        <v>47</v>
+      </c>
+      <c r="U17" s="29">
+        <f>SUM(M17:T17)</f>
+        <v>662</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="24">
+        <v>83</v>
+      </c>
+      <c r="C18" s="24">
+        <v>93</v>
+      </c>
+      <c r="D18" s="24">
+        <v>4</v>
+      </c>
+      <c r="E18" s="24">
+        <v>74</v>
+      </c>
+      <c r="F18" s="24">
+        <v>3</v>
+      </c>
+      <c r="G18" s="24">
+        <v>46</v>
+      </c>
+      <c r="H18" s="24">
+        <v>16</v>
+      </c>
+      <c r="I18" s="24">
+        <v>68</v>
+      </c>
+      <c r="J18" s="19">
+        <f t="shared" ref="J18:J27" si="14">SUM(B18:I18)</f>
+        <v>387</v>
+      </c>
+      <c r="L18" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="24">
+        <f t="shared" ref="M18:M26" si="15">B18*$X4</f>
+        <v>41.5</v>
+      </c>
+      <c r="N18" s="24">
+        <f t="shared" si="13"/>
+        <v>46.5</v>
+      </c>
+      <c r="O18" s="24">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="P18" s="24">
+        <f t="shared" si="13"/>
+        <v>37</v>
+      </c>
+      <c r="Q18" s="24">
+        <f t="shared" si="13"/>
+        <v>1.5</v>
+      </c>
+      <c r="R18" s="24">
+        <f t="shared" si="13"/>
+        <v>23</v>
+      </c>
+      <c r="S18" s="24">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="T18" s="24">
+        <f t="shared" si="13"/>
+        <v>34</v>
+      </c>
+      <c r="U18" s="29">
+        <f t="shared" ref="U18:U26" si="16">SUM(M18:T18)</f>
+        <v>193.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="24">
+        <v>19</v>
+      </c>
+      <c r="C19" s="24">
+        <v>66</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24">
+        <v>85</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24">
+        <v>9</v>
+      </c>
+      <c r="H19" s="24">
+        <v>2</v>
+      </c>
+      <c r="I19" s="24">
+        <v>18</v>
+      </c>
+      <c r="J19" s="19">
+        <f t="shared" si="14"/>
+        <v>199</v>
+      </c>
+      <c r="L19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="24">
+        <f t="shared" si="15"/>
+        <v>19</v>
+      </c>
+      <c r="N19" s="24">
+        <f t="shared" si="13"/>
+        <v>66</v>
+      </c>
+      <c r="O19" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="24">
+        <f t="shared" si="13"/>
+        <v>85</v>
+      </c>
+      <c r="Q19" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="24">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="S19" s="24">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="T19" s="24">
+        <f t="shared" si="13"/>
+        <v>18</v>
+      </c>
+      <c r="U19" s="29">
+        <f t="shared" si="16"/>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="24">
+        <v>1</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="19">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="L20" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="24">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="N20" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S20" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="29">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="24">
+        <v>1</v>
+      </c>
+      <c r="C21" s="24">
+        <v>1</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24">
+        <v>4</v>
+      </c>
+      <c r="F21" s="24">
+        <v>2</v>
+      </c>
+      <c r="G21" s="24">
+        <v>3</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24">
+        <v>3</v>
+      </c>
+      <c r="J21" s="19">
+        <f t="shared" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="24">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="N21" s="24">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="O21" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="24">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="Q21" s="24">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="R21" s="24">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="S21" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T21" s="24">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="U21" s="29">
+        <f t="shared" si="16"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="37"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="24">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S22" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="29">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="24">
+        <v>4</v>
+      </c>
+      <c r="C23" s="24">
+        <v>2</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="19">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="24">
+        <f t="shared" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="N23" s="24">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="O23" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="29">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="37"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36">
+        <v>20</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36">
+        <v>3</v>
+      </c>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36">
+        <v>47</v>
+      </c>
+      <c r="J24" s="19">
+        <f t="shared" si="14"/>
+        <v>70</v>
+      </c>
+      <c r="L24" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" s="24">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="24">
+        <f t="shared" si="13"/>
+        <v>30</v>
+      </c>
+      <c r="Q24" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="24">
+        <f t="shared" si="13"/>
+        <v>4.5</v>
+      </c>
+      <c r="S24" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="24">
+        <f t="shared" si="13"/>
+        <v>70.5</v>
+      </c>
+      <c r="U24" s="29">
+        <f t="shared" si="16"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="24">
+        <v>124</v>
+      </c>
+      <c r="C25" s="24">
+        <v>1</v>
+      </c>
+      <c r="D25" s="24">
+        <v>11</v>
+      </c>
+      <c r="E25" s="24">
+        <v>136</v>
+      </c>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24">
+        <v>96</v>
+      </c>
+      <c r="H25" s="24">
+        <v>59</v>
+      </c>
+      <c r="I25" s="24">
+        <v>66</v>
+      </c>
+      <c r="J25" s="19">
+        <f t="shared" si="14"/>
+        <v>493</v>
+      </c>
+      <c r="L25" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="24">
+        <f t="shared" si="15"/>
+        <v>310</v>
+      </c>
+      <c r="N25" s="24">
+        <f t="shared" si="13"/>
+        <v>2.5</v>
+      </c>
+      <c r="O25" s="24">
+        <f t="shared" si="13"/>
+        <v>27.5</v>
+      </c>
+      <c r="P25" s="24">
+        <f t="shared" si="13"/>
+        <v>340</v>
+      </c>
+      <c r="Q25" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="24">
+        <f t="shared" si="13"/>
+        <v>240</v>
+      </c>
+      <c r="S25" s="24">
+        <f t="shared" si="13"/>
+        <v>147.5</v>
+      </c>
+      <c r="T25" s="24">
+        <f t="shared" si="13"/>
+        <v>165</v>
+      </c>
+      <c r="U25" s="29">
+        <f t="shared" si="16"/>
+        <v>1232.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" s="36">
+        <v>1</v>
+      </c>
+      <c r="D26" s="36">
+        <v>2</v>
+      </c>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36">
+        <v>1</v>
+      </c>
+      <c r="I26" s="36">
+        <v>2</v>
+      </c>
+      <c r="J26" s="19">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="L26" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="24">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="24">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="O26" s="24">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="P26" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S26" s="24">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="T26" s="24">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="U26" s="29">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19">
+        <f>SUM(B17:B26)</f>
+        <v>319</v>
+      </c>
+      <c r="C27" s="19">
+        <f t="shared" ref="C27:I27" si="17">SUM(C17:C26)</f>
+        <v>468</v>
+      </c>
+      <c r="D27" s="19">
+        <f t="shared" si="17"/>
+        <v>24</v>
+      </c>
+      <c r="E27" s="19">
+        <f t="shared" si="17"/>
+        <v>484</v>
+      </c>
+      <c r="F27" s="19">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="19">
+        <f t="shared" si="17"/>
+        <v>202</v>
+      </c>
+      <c r="H27" s="19">
+        <f t="shared" si="17"/>
+        <v>82</v>
+      </c>
+      <c r="I27" s="19">
+        <f t="shared" si="17"/>
+        <v>251</v>
+      </c>
+      <c r="J27" s="19">
+        <f t="shared" si="14"/>
+        <v>1838</v>
+      </c>
+      <c r="M27" s="19">
+        <f>SUM(M17:M26)</f>
+        <v>471.5</v>
+      </c>
+      <c r="N27" s="19">
+        <f t="shared" ref="N27:U27" si="18">SUM(N17:N26)</f>
+        <v>427</v>
+      </c>
+      <c r="O27" s="19">
+        <f t="shared" si="18"/>
+        <v>38.5</v>
+      </c>
+      <c r="P27" s="19">
+        <f t="shared" si="18"/>
+        <v>665</v>
+      </c>
+      <c r="Q27" s="19">
+        <f t="shared" si="18"/>
+        <v>8.5</v>
+      </c>
+      <c r="R27" s="19">
+        <f t="shared" si="18"/>
+        <v>327.5</v>
+      </c>
+      <c r="S27" s="19">
+        <f t="shared" si="18"/>
+        <v>162.5</v>
+      </c>
+      <c r="T27" s="19">
+        <f t="shared" si="18"/>
+        <v>342.5</v>
+      </c>
+      <c r="U27" s="19">
+        <f t="shared" si="18"/>
+        <v>2443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318B7272-D405-4928-809B-51CABE90AAA9}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,8 +5343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D187AD-24A7-4CC8-A4AB-7FAF743362FD}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2285,8 +5855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A804B6F-BEB0-4A34-9EA9-C7A2924BDD35}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2894,8 +6464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618456B1-0405-4E68-A7AA-78422A2C73AA}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3356,7 +6926,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="B16" sqref="B16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3941,7 +7511,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="B16" sqref="B16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4476,7 +8046,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B16" sqref="B16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5066,4 +8636,654 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439BD0BB-2FBB-401D-B7D7-95AD28EF9A5F}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="9" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="19"/>
+      <c r="M1" s="26"/>
+    </row>
+    <row r="2" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22">
+        <v>85</v>
+      </c>
+      <c r="C2" s="23">
+        <v>64</v>
+      </c>
+      <c r="D2" s="23">
+        <v>2</v>
+      </c>
+      <c r="E2" s="23">
+        <v>193</v>
+      </c>
+      <c r="F2" s="23">
+        <v>0</v>
+      </c>
+      <c r="G2" s="23">
+        <v>101</v>
+      </c>
+      <c r="H2" s="23">
+        <v>15</v>
+      </c>
+      <c r="I2" s="23">
+        <v>141</v>
+      </c>
+      <c r="J2" s="23">
+        <f>SUM(B2:I2)</f>
+        <v>601</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="19"/>
+    </row>
+    <row r="3" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22">
+        <v>179</v>
+      </c>
+      <c r="C3" s="23">
+        <v>90</v>
+      </c>
+      <c r="D3" s="23">
+        <v>7</v>
+      </c>
+      <c r="E3" s="23">
+        <v>317</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0</v>
+      </c>
+      <c r="G3" s="23">
+        <v>139</v>
+      </c>
+      <c r="H3" s="23">
+        <v>25</v>
+      </c>
+      <c r="I3" s="23">
+        <v>298</v>
+      </c>
+      <c r="J3" s="23">
+        <f t="shared" ref="J3:J16" si="0">SUM(B3:I3)</f>
+        <v>1055</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22">
+        <v>319</v>
+      </c>
+      <c r="C4" s="23">
+        <v>262</v>
+      </c>
+      <c r="D4" s="23">
+        <v>33</v>
+      </c>
+      <c r="E4" s="23">
+        <v>530</v>
+      </c>
+      <c r="F4" s="23">
+        <v>2</v>
+      </c>
+      <c r="G4" s="23">
+        <v>246</v>
+      </c>
+      <c r="H4" s="23">
+        <v>60</v>
+      </c>
+      <c r="I4" s="23">
+        <v>636</v>
+      </c>
+      <c r="J4" s="23">
+        <f t="shared" si="0"/>
+        <v>2088</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22">
+        <v>544</v>
+      </c>
+      <c r="C5" s="23">
+        <v>308</v>
+      </c>
+      <c r="D5" s="23">
+        <v>41</v>
+      </c>
+      <c r="E5" s="23">
+        <v>733</v>
+      </c>
+      <c r="F5" s="23">
+        <v>8</v>
+      </c>
+      <c r="G5" s="23">
+        <v>378</v>
+      </c>
+      <c r="H5" s="23">
+        <v>86</v>
+      </c>
+      <c r="I5" s="23">
+        <v>654</v>
+      </c>
+      <c r="J5" s="23">
+        <f t="shared" si="0"/>
+        <v>2752</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="19"/>
+    </row>
+    <row r="6" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22">
+        <v>532</v>
+      </c>
+      <c r="C6" s="23">
+        <v>289</v>
+      </c>
+      <c r="D6" s="23">
+        <v>19</v>
+      </c>
+      <c r="E6" s="23">
+        <v>697</v>
+      </c>
+      <c r="F6" s="23">
+        <v>17</v>
+      </c>
+      <c r="G6" s="23">
+        <v>360</v>
+      </c>
+      <c r="H6" s="23">
+        <v>88</v>
+      </c>
+      <c r="I6" s="23">
+        <v>720</v>
+      </c>
+      <c r="J6" s="23">
+        <f t="shared" si="0"/>
+        <v>2722</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+    </row>
+    <row r="7" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22">
+        <v>506</v>
+      </c>
+      <c r="C7" s="23">
+        <v>346</v>
+      </c>
+      <c r="D7" s="23">
+        <v>41</v>
+      </c>
+      <c r="E7" s="23">
+        <v>646</v>
+      </c>
+      <c r="F7" s="23">
+        <v>8</v>
+      </c>
+      <c r="G7" s="23">
+        <v>339</v>
+      </c>
+      <c r="H7" s="23">
+        <v>88</v>
+      </c>
+      <c r="I7" s="23">
+        <v>643</v>
+      </c>
+      <c r="J7" s="23">
+        <f t="shared" si="0"/>
+        <v>2617</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22">
+        <v>503</v>
+      </c>
+      <c r="C8" s="23">
+        <v>314</v>
+      </c>
+      <c r="D8" s="23">
+        <v>35</v>
+      </c>
+      <c r="E8" s="23">
+        <v>701</v>
+      </c>
+      <c r="F8" s="23">
+        <v>9</v>
+      </c>
+      <c r="G8" s="23">
+        <v>380</v>
+      </c>
+      <c r="H8" s="23">
+        <v>115</v>
+      </c>
+      <c r="I8" s="23">
+        <v>615</v>
+      </c>
+      <c r="J8" s="23">
+        <f t="shared" si="0"/>
+        <v>2672</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24">
+        <v>403</v>
+      </c>
+      <c r="C9" s="25">
+        <v>276</v>
+      </c>
+      <c r="D9" s="25">
+        <v>22</v>
+      </c>
+      <c r="E9" s="25">
+        <v>665</v>
+      </c>
+      <c r="F9" s="25">
+        <v>12</v>
+      </c>
+      <c r="G9" s="25">
+        <v>193</v>
+      </c>
+      <c r="H9" s="25">
+        <v>89</v>
+      </c>
+      <c r="I9" s="25">
+        <v>395</v>
+      </c>
+      <c r="J9" s="25">
+        <f t="shared" si="0"/>
+        <v>2055</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24">
+        <v>480</v>
+      </c>
+      <c r="C10" s="25">
+        <v>445</v>
+      </c>
+      <c r="D10" s="25">
+        <v>59</v>
+      </c>
+      <c r="E10" s="25">
+        <v>698</v>
+      </c>
+      <c r="F10" s="25">
+        <v>8</v>
+      </c>
+      <c r="G10" s="25">
+        <v>278</v>
+      </c>
+      <c r="H10" s="25">
+        <v>144</v>
+      </c>
+      <c r="I10" s="25">
+        <v>523</v>
+      </c>
+      <c r="J10" s="25">
+        <f t="shared" si="0"/>
+        <v>2635</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+    </row>
+    <row r="11" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="24">
+        <v>455</v>
+      </c>
+      <c r="C11" s="25">
+        <v>428</v>
+      </c>
+      <c r="D11" s="25">
+        <v>34</v>
+      </c>
+      <c r="E11" s="25">
+        <v>690</v>
+      </c>
+      <c r="F11" s="25">
+        <v>6</v>
+      </c>
+      <c r="G11" s="25">
+        <v>284</v>
+      </c>
+      <c r="H11" s="25">
+        <v>127</v>
+      </c>
+      <c r="I11" s="25">
+        <v>544</v>
+      </c>
+      <c r="J11" s="25">
+        <f t="shared" si="0"/>
+        <v>2568</v>
+      </c>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+    </row>
+    <row r="12" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="24">
+        <v>529</v>
+      </c>
+      <c r="C12" s="25">
+        <v>430</v>
+      </c>
+      <c r="D12" s="25">
+        <v>42</v>
+      </c>
+      <c r="E12" s="25">
+        <v>742</v>
+      </c>
+      <c r="F12" s="25">
+        <v>11</v>
+      </c>
+      <c r="G12" s="25">
+        <v>355</v>
+      </c>
+      <c r="H12" s="25">
+        <v>123</v>
+      </c>
+      <c r="I12" s="25">
+        <v>486</v>
+      </c>
+      <c r="J12" s="25">
+        <f t="shared" si="0"/>
+        <v>2718</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" s="19"/>
+    </row>
+    <row r="13" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="24">
+        <v>510</v>
+      </c>
+      <c r="C13" s="25">
+        <v>481</v>
+      </c>
+      <c r="D13" s="25">
+        <v>33</v>
+      </c>
+      <c r="E13" s="25">
+        <v>593</v>
+      </c>
+      <c r="F13" s="25">
+        <v>11</v>
+      </c>
+      <c r="G13" s="25">
+        <v>350</v>
+      </c>
+      <c r="H13" s="25">
+        <v>120</v>
+      </c>
+      <c r="I13" s="25">
+        <v>474</v>
+      </c>
+      <c r="J13" s="25">
+        <f t="shared" si="0"/>
+        <v>2572</v>
+      </c>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+    </row>
+    <row r="14" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="24">
+        <v>540</v>
+      </c>
+      <c r="C14" s="25">
+        <v>573</v>
+      </c>
+      <c r="D14" s="25">
+        <v>33</v>
+      </c>
+      <c r="E14" s="25">
+        <v>647</v>
+      </c>
+      <c r="F14" s="25">
+        <v>12</v>
+      </c>
+      <c r="G14" s="25">
+        <v>298</v>
+      </c>
+      <c r="H14" s="25">
+        <v>107</v>
+      </c>
+      <c r="I14" s="25">
+        <v>462</v>
+      </c>
+      <c r="J14" s="25">
+        <f t="shared" si="0"/>
+        <v>2672</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+    </row>
+    <row r="15" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="24">
+        <v>493</v>
+      </c>
+      <c r="C15" s="25">
+        <v>546</v>
+      </c>
+      <c r="D15" s="25">
+        <v>36</v>
+      </c>
+      <c r="E15" s="25">
+        <v>668</v>
+      </c>
+      <c r="F15" s="25">
+        <v>10</v>
+      </c>
+      <c r="G15" s="25">
+        <v>254</v>
+      </c>
+      <c r="H15" s="25">
+        <v>97</v>
+      </c>
+      <c r="I15" s="25">
+        <v>432</v>
+      </c>
+      <c r="J15" s="25">
+        <f t="shared" si="0"/>
+        <v>2536</v>
+      </c>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="24">
+        <v>319</v>
+      </c>
+      <c r="C16" s="25">
+        <v>468</v>
+      </c>
+      <c r="D16" s="25">
+        <v>24</v>
+      </c>
+      <c r="E16" s="25">
+        <v>484</v>
+      </c>
+      <c r="F16" s="25">
+        <v>8</v>
+      </c>
+      <c r="G16" s="25">
+        <v>202</v>
+      </c>
+      <c r="H16" s="25">
+        <v>82</v>
+      </c>
+      <c r="I16" s="25">
+        <v>251</v>
+      </c>
+      <c r="J16" s="25">
+        <f t="shared" si="0"/>
+        <v>1838</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="19">
+        <f>LARGE(J2:J8,1)</f>
+        <v>2752</v>
+      </c>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="19">
+        <f>SMALL(J2:J8,1)</f>
+        <v>601</v>
+      </c>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H19" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="19">
+        <f>LARGE(J9:J16,1)</f>
+        <v>2718</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I20" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="19">
+        <f>SMALL(J9:J16,1)</f>
+        <v>1838</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>